<commit_message>
change: example SingleSetup and docstrings
</commit_message>
<xml_diff>
--- a/src/pyoma2/test_data/palisaden/Geo1.xlsx
+++ b/src/pyoma2/test_data/palisaden/Geo1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://treteknisk-my.sharepoint.com/personal/dpa_treteknisk_no/Documents/Dokumenter/Dev/pyOMA2/src/pyoma2/test_data/palisaden/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{251A879C-2DC2-4A73-B0CD-F5AB25CF734A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{251A879C-2DC2-4A73-B0CD-F5AB25CF734A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{439BA47B-F2A9-4E88-9AFD-0A4902D0AC4F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{239D3FD3-7DB5-43CA-A3A1-49071C9EC557}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{239D3FD3-7DB5-43CA-A3A1-49071C9EC557}"/>
   </bookViews>
   <sheets>
     <sheet name="sensors names" sheetId="19" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>x</t>
   </si>
@@ -66,21 +66,6 @@
     <t>z</t>
   </si>
   <si>
-    <t>ch1_1</t>
-  </si>
-  <si>
-    <t>ch2_1</t>
-  </si>
-  <si>
-    <t>ch3_1</t>
-  </si>
-  <si>
-    <t>ch4_1</t>
-  </si>
-  <si>
-    <t>ch5_1</t>
-  </si>
-  <si>
     <t>setup No.</t>
   </si>
   <si>
@@ -108,7 +93,28 @@
     <t>end</t>
   </si>
   <si>
-    <t>na</t>
+    <t>chann. 6</t>
+  </si>
+  <si>
+    <t>ch1</t>
+  </si>
+  <si>
+    <t>ch2</t>
+  </si>
+  <si>
+    <t>ch3</t>
+  </si>
+  <si>
+    <t>ch4</t>
+  </si>
+  <si>
+    <t>ch5</t>
+  </si>
+  <si>
+    <t>ch6</t>
+  </si>
+  <si>
+    <t>ptName</t>
   </si>
 </sst>
 </file>
@@ -187,9 +193,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +233,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -333,7 +339,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B5F60D-4600-45C6-9F9B-CE573204C65F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="K4" sqref="K4:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,44 +501,50 @@
     <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -543,10 +555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63EEFAF-45DA-4A18-AEC3-F6C99055E21F}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,9 +567,9 @@
     <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -569,88 +581,91 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
       <c r="C7" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -660,10 +675,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8647A2-283F-45ED-8CDC-E05E1BE90853}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,9 +687,9 @@
     <col min="2" max="16384" width="5.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -686,89 +701,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -777,10 +795,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B519F1-6E02-432D-A33C-937A98D77CCB}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,60 +806,17 @@
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -853,7 +828,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +839,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -877,84 +852,84 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
+      <c r="A3" s="1">
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
+      <c r="A4" s="1">
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="1">
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
+      <c r="A6" s="1">
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
+      <c r="A7" s="1">
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -970,10 +945,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59F39B5-D487-4E58-BF61-A925B720FB4E}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,68 +958,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>